<commit_message>
04.09.25 9.49AM new test case added for coupon
</commit_message>
<xml_diff>
--- a/reports/Extent-Report/Zlaata-QAResults.xlsx
+++ b/reports/Extent-Report/Zlaata-QAResults.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="111">
   <si>
     <t>Duration</t>
   </si>
@@ -229,114 +229,135 @@
     <t>DEVICE NAME</t>
   </si>
   <si>
-    <t>Sept 02, 2025 5:52:51 pm</t>
-  </si>
-  <si>
-    <t>Sept 02, 2025 5:50:48 pm</t>
-  </si>
-  <si>
-    <t>Sept 02, 2025 5:52:50 pm</t>
-  </si>
-  <si>
-    <t>2 m 1.707 s</t>
+    <t>Sept 04, 2025 9:41:05 am</t>
+  </si>
+  <si>
+    <t>Sept 04, 2025 9:33:15 am</t>
+  </si>
+  <si>
+    <t>Sept 04, 2025 9:41:03 am</t>
+  </si>
+  <si>
+    <t>7 m 47.319 s</t>
   </si>
   <si>
     <t>0%</t>
   </si>
   <si>
-    <t>33%</t>
+    <t>70%</t>
+  </si>
+  <si>
+    <t>@TC_UI_Zlaata_COP_06</t>
+  </si>
+  <si>
+    <t>@TC_UI_Zlaata_COP_07</t>
+  </si>
+  <si>
+    <t>@TC_UI_Zlaata_COP_09</t>
+  </si>
+  <si>
+    <t>CheckOut Page Feature</t>
+  </si>
+  <si>
+    <t>TC_UI_Zlaata_COP_06 |Verify User Can Add New Product|"TD_UI_Zlaata_COP_06"</t>
+  </si>
+  <si>
+    <t>TC_UI_Zlaata_COP_07 |Verify That Adding Product to Bag Count is Displaying or Not Above Bag Icon|"TD_UI_Zlaata_COP_07"</t>
+  </si>
+  <si>
+    <t>TC_UI_Zlaata_COP_09 |Verify That Calculation Functionality is Working|"TD_UI_Zlaata_COP_09"</t>
+  </si>
+  <si>
+    <t>TC_UI_Zlaata_COP_01 |Verify Bag Item Count Display|"TD_UI_Zlaata_COP_01"</t>
+  </si>
+  <si>
+    <t>30.759 s</t>
+  </si>
+  <si>
+    <t>TC_UI_Zlaata_COP_02 |Verify Display of Wishlist Button|"TD_UI_Zlaata_COP_02"</t>
+  </si>
+  <si>
+    <t>56.156 s</t>
+  </si>
+  <si>
+    <t>TC_UI_Zlaata_COP_03 |Verify Display of Delete Button|"TD_UI_Zlaata_COP_03"</t>
+  </si>
+  <si>
+    <t>53.592 s</t>
+  </si>
+  <si>
+    <t>TC_UI_Zlaata_COP_04 |Verify That User Can Change Product Size|"TD_UI_Zlaata_COP_04"</t>
+  </si>
+  <si>
+    <t>1 m 4.945 s</t>
+  </si>
+  <si>
+    <t>TC_UI_Zlaata_COP_05 |Verify User Can Increase or Decrease Product Quantity|"TD_UI_Zlaata_COP_05"</t>
+  </si>
+  <si>
+    <t>59.585 s</t>
+  </si>
+  <si>
+    <t>46.215 s</t>
+  </si>
+  <si>
+    <t>0.903 s</t>
+  </si>
+  <si>
+    <t>TC_UI_Zlaata_COP_08 |Verify That Adding New Product or Deleting Product Count Increases or Decreases|"TD_UI_Zlaata_COP_08"</t>
+  </si>
+  <si>
+    <t>1 m 39.929 s</t>
+  </si>
+  <si>
+    <t>0.932 s</t>
+  </si>
+  <si>
+    <t>TC_UI_Zlaata_COP_10 |Verify Accessories, Recently Viewed, and Top Selling buttons on Checkout page| "TD_UI_Zlaata_COP_10"</t>
+  </si>
+  <si>
+    <t>53.631 s</t>
   </si>
   <si>
     <t>@TC_UI_Zlaata_COP_01</t>
   </si>
   <si>
+    <t>100%</t>
+  </si>
+  <si>
     <t>@TC_UI_Zlaata_COP_02</t>
   </si>
   <si>
-    <t>CheckOut Page Feature</t>
-  </si>
-  <si>
-    <t>TC_UI_Zlaata_COP_01 |Verify Bag Item Count Display|"TD_UI_Zlaata_COP_01"</t>
-  </si>
-  <si>
-    <t>TC_UI_Zlaata_COP_02 |Verify Display of Wishlist Button|"TD_UI_Zlaata_COP_02"</t>
-  </si>
-  <si>
-    <t>1 m 4.692 s</t>
-  </si>
-  <si>
-    <t>45.166 s</t>
-  </si>
-  <si>
-    <t>TC_UI_Zlaata_COP_03 |Verify Display of Delete Button|"TD_UI_Zlaata_COP_03"</t>
-  </si>
-  <si>
-    <t>11.275 s</t>
-  </si>
-  <si>
     <t>@TC_UI_Zlaata_COP_03</t>
   </si>
   <si>
-    <t>100%</t>
-  </si>
-  <si>
-    <t>2 m 1.174 s</t>
-  </si>
-  <si>
-    <t>Given User Verifies Bag Item Count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org.openqa.selenium.ElementNotInteractableException: element not interactable
-  (Session info: chrome=139.0.7258.155)
-Build info: version: '4.34.0', revision: '707dcb4246*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '22.0.1'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [be5b5703f1d91ce1e879dbfa92367ee6, clickElement {id=f.94D8FB993CDB9B9134B96C8217780AD5.d.846233820477408E60DDEBB4BF725884.e.99}]
-Capabilities {acceptInsecureCerts: true, browserName: chrome, browserVersion: 139.0.7258.155, chrome: {chromedriverVersion: 139.0.7258.154 (9e0d6b2b47f..., userDataDir: C:\Users\Ranjith\AppData\Lo...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:61333}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:61333/devtoo..., se:cdpVersion: 139.0.7258.155, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Element: [[ChromeDriver: chrome on windows (be5b5703f1d91ce1e879dbfa92367ee6)] -&gt; xpath: //button[text()='Submit']]
-Session ID: be5b5703f1d91ce1e879dbfa92367ee6
-	at java.base/jdk.internal.reflect.DirectConstructorHandleAccessor.newInstance(DirectConstructorHandleAccessor.java:62)
-	at java.base/java.lang.reflect.Constructor.newInstanceWithCaller(Constructor.java:502)
-	at java.base/java.lang.reflect.Constructor.newInstance(Constructor.java:486)
-	at org.openqa.selenium.remote.ErrorCodec.decode(ErrorCodec.java:167)
-	at org.openqa.selenium.remote.codec.w3c.W3CHttpResponseCodec.decode(W3CHttpResponseCodec.java:138)
-	at org.openqa.selenium.remote.codec.w3c.W3CHttpResponseCodec.decode(W3CHttpResponseCodec.java:50)
-	at org.openqa.selenium.remote.HttpCommandExecutor.execute(HttpCommandExecutor.java:215)
-	at org.openqa.selenium.remote.service.DriverCommandExecutor.invokeExecute(DriverCommandExecutor.java:216)
-	at org.openqa.selenium.remote.service.DriverCommandExecutor.execute(DriverCommandExecutor.java:174)
-	at org.openqa.selenium.remote.RemoteWebDriver.execute(RemoteWebDriver.java:544)
-	at org.openqa.selenium.remote.RemoteWebElement.execute(RemoteWebElement.java:223)
-	at org.openqa.selenium.remote.RemoteWebElement.click(RemoteWebElement.java:76)
-	at java.base/jdk.internal.reflect.DirectMethodHandleAccessor.invoke(DirectMethodHandleAccessor.java:103)
-	at java.base/java.lang.reflect.Method.invoke(Method.java:580)
-	at org.openqa.selenium.support.decorators.WebDriverDecorator.call(WebDriverDecorator.java:315)
-	at org.openqa.selenium.support.decorators.DefaultDecorated.call(DefaultDecorated.java:48)
-	at org.openqa.selenium.support.decorators.WebDriverDecorator.lambda$createProxyFactory$3(WebDriverDecorator.java:405)
-	at net.bytebuddy.renamed.java.lang.Object$ByteBuddy$2WLj8y6O.click(Unknown Source)
-	at java.base/jdk.internal.reflect.DirectMethodHandleAccessor.invoke(DirectMethodHandleAccessor.java:103)
-	at java.base/java.lang.reflect.Method.invoke(Method.java:580)
-	at org.openqa.selenium.support.pagefactory.internal.LocatingElementHandler.invoke(LocatingElementHandler.java:51)
-	at jdk.proxy2/jdk.proxy2.$Proxy50.click(Unknown Source)
-	at basePage.BasePage.click(BasePage.java:78)
-	at pages.HomePage.homeLaunch(HomePage.java:34)
-	at pages.CheckoutPage.itemCount(CheckoutPage.java:426)
-	at stepDef.CheckOutPageStepDef.user_verifies_bag_item_count(CheckOutPageStepDef.java:33)
-	at ✽.User Verifies Bag Item Count(file:///C:/Users/Ranjith/git/zlaataautomation-pixel/zlaata/zlaata/src/test/resources/features/CheckoutPage/checkoutPage.feature:13)
-</t>
-  </si>
-  <si>
-    <t>Given User Verifies Display of Wishlist Button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"//button[@class='Cls_cart_btn Cls_redirect_restrict']"}
+    <t>@TC_UI_Zlaata_COP_04</t>
+  </si>
+  <si>
+    <t>@TC_UI_Zlaata_COP_05</t>
+  </si>
+  <si>
+    <t>@TC_UI_Zlaata_COP_08</t>
+  </si>
+  <si>
+    <t>@TC_UI_Zlaata_COP_10</t>
+  </si>
+  <si>
+    <t>7 m 46.788 s</t>
+  </si>
+  <si>
+    <t>Given User Verifies User Can Add New Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"//button[@class='add_bag_prod_buy_now_btn btn___2 Cls_CartList ClsProductListSizes']"}
   (Session info: chrome=139.0.7258.155)
 For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
 Build info: version: '4.34.0', revision: '707dcb4246*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '22.0.1'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [5120a948146cdb15a9cb14351b3d069b, findElement {value=//button[@class='Cls_cart_btn Cls_redirect_restrict'], using=xpath}]
-Capabilities {acceptInsecureCerts: true, browserName: chrome, browserVersion: 139.0.7258.155, chrome: {chromedriverVersion: 139.0.7258.154 (9e0d6b2b47f..., userDataDir: C:\Users\Ranjith\AppData\Lo...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:53494}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:53494/devtoo..., se:cdpVersion: 139.0.7258.155, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: 5120a948146cdb15a9cb14351b3d069b
+Command: [370a4f509e6f398047521b0010f3b005, findElement {using=xpath, value=//button[@class='add_bag_prod_buy_now_btn btn___2 Cls_CartList ClsProductListSizes']}]
+Capabilities {acceptInsecureCerts: true, browserName: chrome, browserVersion: 139.0.7258.155, chrome: {chromedriverVersion: 139.0.7258.154 (9e0d6b2b47f..., userDataDir: C:\Users\GOWTHA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:51169}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:51169/devtoo..., se:cdpVersion: 139.0.7258.155, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 370a4f509e6f398047521b0010f3b005
 	at java.base/jdk.internal.reflect.DirectConstructorHandleAccessor.newInstance(DirectConstructorHandleAccessor.java:62)
 	at java.base/java.lang.reflect.Constructor.newInstanceWithCaller(Constructor.java:502)
 	at java.base/java.lang.reflect.Constructor.newInstance(Constructor.java:486)
@@ -356,14 +377,32 @@
 	at org.openqa.selenium.support.decorators.WebDriverDecorator.call(WebDriverDecorator.java:315)
 	at org.openqa.selenium.support.decorators.DefaultDecorated.call(DefaultDecorated.java:48)
 	at org.openqa.selenium.support.decorators.WebDriverDecorator.lambda$createProxyFactory$3(WebDriverDecorator.java:405)
-	at net.bytebuddy.renamed.java.lang.Object$ByteBuddy$Nd7pTPUF.findElement(Unknown Source)
+	at net.bytebuddy.renamed.java.lang.Object$ByteBuddy$KnqGqlbp.findElement(Unknown Source)
 	at org.openqa.selenium.support.pagefactory.DefaultElementLocator.findElement(DefaultElementLocator.java:68)
 	at org.openqa.selenium.support.pagefactory.internal.LocatingElementHandler.invoke(LocatingElementHandler.java:38)
 	at jdk.proxy2/jdk.proxy2.$Proxy50.click(Unknown Source)
 	at basePage.BasePage.click(BasePage.java:78)
-	at pages.CheckoutPage.wishListInbag(CheckoutPage.java:459)
-	at stepDef.CheckOutPageStepDef.user_verifies_display_of_wishlist_button(CheckOutPageStepDef.java:41)
-	at ✽.User Verifies Display of Wishlist Button(file:///C:/Users/Ranjith/git/zlaataautomation-pixel/zlaata/zlaata/src/test/resources/features/CheckoutPage/checkoutPage.feature:22)
+	at pages.ProductListingPage.addToCart(ProductListingPage.java:437)
+	at pages.CheckoutPage.newProductToBag(CheckoutPage.java:774)
+	at stepDef.CheckOutPageStepDef.user_verifies_user_can_add_new_product(CheckOutPageStepDef.java:71)
+	at ✽.User Verifies User Can Add New Product(file:///C:/Users/gowthamraj/git/zlaatanew/src/test/resources/features/CheckoutPage/checkoutPage.feature:54)
+</t>
+  </si>
+  <si>
+    <t>Given User Verifies That Adding Product to Bag Count is Displaying or Not Above Bag Icon</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>stepDef.Hooks.preCondition(io.cucumber.java.Scenario)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">java.lang.NullPointerException: Cannot invoke "java.util.Map.get(Object)" because "dataMap" is null
+	at utils.Common.getValueFromHashMap(Common.java:69)
+	at utils.ExcelUtils.writeToExcel(ExcelUtils.java:65)
+	at dataProviders.TestData.getTestData(TestData.java:104)
+	at stepDef.Hooks.preCondition(Hooks.java:102)
 </t>
   </si>
 </sst>
@@ -506,6 +545,12 @@
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
+      <color rgb="00FF00"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <i val="true"/>
     </font>
     <font>
@@ -522,12 +567,6 @@
       <name val="Calibri"/>
       <sz val="11.0"/>
       <color rgb="FFFF00"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color rgb="00FF00"/>
-      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -826,7 +865,7 @@
       <alignment vertical="top" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
-      <alignment vertical="top" wrapText="true" horizontal="center"/>
+      <alignment vertical="top" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
       <alignment vertical="top" wrapText="true" horizontal="center"/>
@@ -835,7 +874,7 @@
       <alignment vertical="top" wrapText="true" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
-      <alignment vertical="top" wrapText="true"/>
+      <alignment vertical="top" wrapText="true" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
       <alignment vertical="top" wrapText="true" horizontal="center"/>
@@ -981,21 +1020,24 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'DB Data'!$A$20:$A$21</c:f>
+              <c:f>'DB Data'!$A$20:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>@TC_UI_Zlaata_COP_01</c:v>
+                  <c:v>@TC_UI_Zlaata_COP_06</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>@TC_UI_Zlaata_COP_02</c:v>
+                  <c:v>@TC_UI_Zlaata_COP_07</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>@TC_UI_Zlaata_COP_09</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'DB Data'!$B$20:$B$21</c:f>
+              <c:f>'DB Data'!$B$20:$B$22</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -1052,21 +1094,24 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'DB Data'!$A$20:$A$21</c:f>
+              <c:f>'DB Data'!$A$20:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>@TC_UI_Zlaata_COP_01</c:v>
+                  <c:v>@TC_UI_Zlaata_COP_06</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>@TC_UI_Zlaata_COP_02</c:v>
+                  <c:v>@TC_UI_Zlaata_COP_07</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>@TC_UI_Zlaata_COP_09</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'DB Data'!$D$20:$D$21</c:f>
+              <c:f>'DB Data'!$D$20:$D$22</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -1123,27 +1168,33 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'DB Data'!$A$20:$A$21</c:f>
+              <c:f>'DB Data'!$A$20:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>@TC_UI_Zlaata_COP_01</c:v>
+                  <c:v>@TC_UI_Zlaata_COP_06</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>@TC_UI_Zlaata_COP_02</c:v>
+                  <c:v>@TC_UI_Zlaata_COP_07</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>@TC_UI_Zlaata_COP_09</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'DB Data'!$C$20:$C$21</c:f>
+              <c:f>'DB Data'!$C$20:$C$22</c:f>
               <c:numCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1371,7 +1422,7 @@
               <c:numCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1510,7 +1561,7 @@
               <c:numCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2675,7 +2726,7 @@
               <c:numCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2814,7 +2865,7 @@
               <c:numCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3028,21 +3079,24 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'DB Data'!$P$20:$P$21</c:f>
+              <c:f>'DB Data'!$P$20:$P$22</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>TC_UI_Zlaata_COP_01 |Verify Bag Item Count Display|"TD_UI_Zlaata_COP_01"</c:v>
+                  <c:v>TC_UI_Zlaata_COP_06 |Verify User Can Add New Product|"TD_UI_Zlaata_COP_06"</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>TC_UI_Zlaata_COP_02 |Verify Display of Wishlist Button|"TD_UI_Zlaata_COP_02"</c:v>
+                  <c:v>TC_UI_Zlaata_COP_07 |Verify That Adding Product to Bag Count is Displaying or Not Above Bag Icon|"TD_UI_Zlaata_COP_07"</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>TC_UI_Zlaata_COP_09 |Verify That Calculation Functionality is Working|"TD_UI_Zlaata_COP_09"</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'DB Data'!$R$20:$R$21</c:f>
+              <c:f>'DB Data'!$R$20:$R$22</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -3098,22 +3152,30 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'DB Data'!$P$20:$P$21</c:f>
+              <c:f>'DB Data'!$P$20:$P$22</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>TC_UI_Zlaata_COP_01 |Verify Bag Item Count Display|"TD_UI_Zlaata_COP_01"</c:v>
+                  <c:v>TC_UI_Zlaata_COP_06 |Verify User Can Add New Product|"TD_UI_Zlaata_COP_06"</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>TC_UI_Zlaata_COP_02 |Verify Display of Wishlist Button|"TD_UI_Zlaata_COP_02"</c:v>
+                  <c:v>TC_UI_Zlaata_COP_07 |Verify That Adding Product to Bag Count is Displaying or Not Above Bag Icon|"TD_UI_Zlaata_COP_07"</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>TC_UI_Zlaata_COP_09 |Verify That Calculation Functionality is Working|"TD_UI_Zlaata_COP_09"</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'DB Data'!$T$20:$T$21</c:f>
-              <c:numCache/>
+              <c:f>'DB Data'!$T$20:$T$22</c:f>
+              <c:numCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -3168,23 +3230,26 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'DB Data'!$P$20:$P$21</c:f>
+              <c:f>'DB Data'!$P$20:$P$22</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>TC_UI_Zlaata_COP_01 |Verify Bag Item Count Display|"TD_UI_Zlaata_COP_01"</c:v>
+                  <c:v>TC_UI_Zlaata_COP_06 |Verify User Can Add New Product|"TD_UI_Zlaata_COP_06"</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>TC_UI_Zlaata_COP_02 |Verify Display of Wishlist Button|"TD_UI_Zlaata_COP_02"</c:v>
+                  <c:v>TC_UI_Zlaata_COP_07 |Verify That Adding Product to Bag Count is Displaying or Not Above Bag Icon|"TD_UI_Zlaata_COP_07"</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>TC_UI_Zlaata_COP_09 |Verify That Calculation Functionality is Working|"TD_UI_Zlaata_COP_09"</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'DB Data'!$S$20:$S$21</c:f>
+              <c:f>'DB Data'!$S$20:$S$22</c:f>
               <c:numCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -4153,9 +4218,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Scenarios!$B$22:$B$24</c:f>
+              <c:f>Scenarios!$B$22:$B$31</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>TC_UI_Zlaata_COP_01 |Verify Bag Item Count Display|"TD_UI_Zlaata_COP_01"</c:v>
                 </c:pt>
@@ -4164,16 +4229,55 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>TC_UI_Zlaata_COP_03 |Verify Display of Delete Button|"TD_UI_Zlaata_COP_03"</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TC_UI_Zlaata_COP_04 |Verify That User Can Change Product Size|"TD_UI_Zlaata_COP_04"</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>TC_UI_Zlaata_COP_05 |Verify User Can Increase or Decrease Product Quantity|"TD_UI_Zlaata_COP_05"</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>TC_UI_Zlaata_COP_06 |Verify User Can Add New Product|"TD_UI_Zlaata_COP_06"</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>TC_UI_Zlaata_COP_07 |Verify That Adding Product to Bag Count is Displaying or Not Above Bag Icon|"TD_UI_Zlaata_COP_07"</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>TC_UI_Zlaata_COP_08 |Verify That Adding New Product or Deleting Product Count Increases or Decreases|"TD_UI_Zlaata_COP_08"</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>TC_UI_Zlaata_COP_09 |Verify That Calculation Functionality is Working|"TD_UI_Zlaata_COP_09"</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>TC_UI_Zlaata_COP_10 |Verify Accessories, Recently Viewed, and Top Selling buttons on Checkout page| "TD_UI_Zlaata_COP_10"</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scenarios!$H$22:$H$24</c:f>
+              <c:f>Scenarios!$H$22:$H$31</c:f>
               <c:numCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
                 <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4231,9 +4335,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Scenarios!$B$22:$B$24</c:f>
+              <c:f>Scenarios!$B$22:$B$31</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>TC_UI_Zlaata_COP_01 |Verify Bag Item Count Display|"TD_UI_Zlaata_COP_01"</c:v>
                 </c:pt>
@@ -4242,14 +4346,40 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>TC_UI_Zlaata_COP_03 |Verify Display of Delete Button|"TD_UI_Zlaata_COP_03"</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TC_UI_Zlaata_COP_04 |Verify That User Can Change Product Size|"TD_UI_Zlaata_COP_04"</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>TC_UI_Zlaata_COP_05 |Verify User Can Increase or Decrease Product Quantity|"TD_UI_Zlaata_COP_05"</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>TC_UI_Zlaata_COP_06 |Verify User Can Add New Product|"TD_UI_Zlaata_COP_06"</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>TC_UI_Zlaata_COP_07 |Verify That Adding Product to Bag Count is Displaying or Not Above Bag Icon|"TD_UI_Zlaata_COP_07"</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>TC_UI_Zlaata_COP_08 |Verify That Adding New Product or Deleting Product Count Increases or Decreases|"TD_UI_Zlaata_COP_08"</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>TC_UI_Zlaata_COP_09 |Verify That Calculation Functionality is Working|"TD_UI_Zlaata_COP_09"</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>TC_UI_Zlaata_COP_10 |Verify Accessories, Recently Viewed, and Top Selling buttons on Checkout page| "TD_UI_Zlaata_COP_10"</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scenarios!$J$22:$J$24</c:f>
-              <c:numCache/>
+              <c:f>Scenarios!$J$22:$J$31</c:f>
+              <c:numCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -4304,9 +4434,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Scenarios!$B$22:$B$24</c:f>
+              <c:f>Scenarios!$B$22:$B$31</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>TC_UI_Zlaata_COP_01 |Verify Bag Item Count Display|"TD_UI_Zlaata_COP_01"</c:v>
                 </c:pt>
@@ -4315,19 +4445,40 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>TC_UI_Zlaata_COP_03 |Verify Display of Delete Button|"TD_UI_Zlaata_COP_03"</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TC_UI_Zlaata_COP_04 |Verify That User Can Change Product Size|"TD_UI_Zlaata_COP_04"</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>TC_UI_Zlaata_COP_05 |Verify User Can Increase or Decrease Product Quantity|"TD_UI_Zlaata_COP_05"</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>TC_UI_Zlaata_COP_06 |Verify User Can Add New Product|"TD_UI_Zlaata_COP_06"</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>TC_UI_Zlaata_COP_07 |Verify That Adding Product to Bag Count is Displaying or Not Above Bag Icon|"TD_UI_Zlaata_COP_07"</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>TC_UI_Zlaata_COP_08 |Verify That Adding New Product or Deleting Product Count Increases or Decreases|"TD_UI_Zlaata_COP_08"</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>TC_UI_Zlaata_COP_09 |Verify That Calculation Functionality is Working|"TD_UI_Zlaata_COP_09"</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>TC_UI_Zlaata_COP_10 |Verify Accessories, Recently Viewed, and Top Selling buttons on Checkout page| "TD_UI_Zlaata_COP_10"</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scenarios!$I$22:$I$24</c:f>
+              <c:f>Scenarios!$I$22:$I$31</c:f>
               <c:numCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="5">
                   <c:v>1.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4729,9 +4880,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tags!$B$22:$B$24</c:f>
+              <c:f>Tags!$B$22:$B$31</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>@TC_UI_Zlaata_COP_01</c:v>
                 </c:pt>
@@ -4740,16 +4891,55 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>@TC_UI_Zlaata_COP_03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>@TC_UI_Zlaata_COP_04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>@TC_UI_Zlaata_COP_05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>@TC_UI_Zlaata_COP_06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>@TC_UI_Zlaata_COP_07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>@TC_UI_Zlaata_COP_08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>@TC_UI_Zlaata_COP_09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>@TC_UI_Zlaata_COP_10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tags!$D$22:$D$24</c:f>
+              <c:f>Tags!$D$22:$D$31</c:f>
               <c:numCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
                 <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4807,9 +4997,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tags!$B$22:$B$24</c:f>
+              <c:f>Tags!$B$22:$B$31</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>@TC_UI_Zlaata_COP_01</c:v>
                 </c:pt>
@@ -4818,13 +5008,34 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>@TC_UI_Zlaata_COP_03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>@TC_UI_Zlaata_COP_04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>@TC_UI_Zlaata_COP_05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>@TC_UI_Zlaata_COP_06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>@TC_UI_Zlaata_COP_07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>@TC_UI_Zlaata_COP_08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>@TC_UI_Zlaata_COP_09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>@TC_UI_Zlaata_COP_10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tags!$F$22:$F$24</c:f>
+              <c:f>Tags!$F$22:$F$31</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -4880,9 +5091,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tags!$B$22:$B$24</c:f>
+              <c:f>Tags!$B$22:$B$31</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>@TC_UI_Zlaata_COP_01</c:v>
                 </c:pt>
@@ -4891,19 +5102,43 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>@TC_UI_Zlaata_COP_03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>@TC_UI_Zlaata_COP_04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>@TC_UI_Zlaata_COP_05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>@TC_UI_Zlaata_COP_06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>@TC_UI_Zlaata_COP_07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>@TC_UI_Zlaata_COP_08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>@TC_UI_Zlaata_COP_09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>@TC_UI_Zlaata_COP_10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tags!$E$22:$E$24</c:f>
+              <c:f>Tags!$E$22:$E$31</c:f>
               <c:numCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="5">
                   <c:v>1.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -5047,13 +5282,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>38099</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1095375</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5079,13 +5314,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1181100</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8567,7 +8802,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B19:G64"/>
+  <dimension ref="B19:G66"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -8611,12 +8846,12 @@
         <v>72</v>
       </c>
       <c r="C39" s="52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D39" s="49"/>
       <c r="E39" s="49"/>
       <c r="F39" s="52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G39" s="53" t="s">
         <v>40</v>
@@ -8627,66 +8862,70 @@
         <v>73</v>
       </c>
       <c r="C40" s="52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D40" s="49"/>
       <c r="E40" s="49"/>
       <c r="F40" s="52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G40" s="53" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
+    <row r="41">
+      <c r="B41" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="G41" s="53" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="61" spans="2:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B61" s="7" t="s">
+    <row r="42" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+    </row>
+    <row r="62" spans="2:7" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B62" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B62" s="36" t="s">
+    <row r="63" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B63" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C62" s="38"/>
-      <c r="D62" s="8" t="s">
+      <c r="C63" s="38"/>
+      <c r="D63" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E62" s="36" t="s">
+      <c r="E63" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="F62" s="38"/>
-      <c r="G62" s="8" t="s">
+      <c r="F63" s="38"/>
+      <c r="G63" s="8" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="B63" s="52" t="s">
-        <v>74</v>
-      </c>
-      <c r="C63" s="49"/>
-      <c r="D63" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="E63" s="52" t="s">
-        <v>75</v>
-      </c>
-      <c r="F63" s="49"/>
-      <c r="G63" s="53" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="64">
-      <c r="B64" s="49"/>
+      <c r="B64" s="52" t="s">
+        <v>75</v>
+      </c>
       <c r="C64" s="49"/>
-      <c r="D64" s="49"/>
+      <c r="D64" s="53" t="s">
+        <v>40</v>
+      </c>
       <c r="E64" s="52" t="s">
         <v>76</v>
       </c>
@@ -8695,18 +8934,44 @@
         <v>40</v>
       </c>
     </row>
+    <row r="65">
+      <c r="B65" s="49"/>
+      <c r="C65" s="49"/>
+      <c r="D65" s="49"/>
+      <c r="E65" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="F65" s="49"/>
+      <c r="G65" s="53" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" s="49"/>
+      <c r="C66" s="49"/>
+      <c r="D66" s="49"/>
+      <c r="E66" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="F66" s="49"/>
+      <c r="G66" s="53" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection sheet="true" password="F883" scenarios="true" objects="true"/>
-  <mergeCells count="11">
+  <sheetProtection sheet="true" password="DB29" scenarios="true" objects="true"/>
+  <mergeCells count="13">
     <mergeCell ref="C38:E38"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="E63:F63"/>
     <mergeCell ref="C39:E39"/>
     <mergeCell ref="C40:E40"/>
-    <mergeCell ref="B63:C64"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="B64:C66"/>
+    <mergeCell ref="D64:D66"/>
     <mergeCell ref="E64:F64"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="E66:F66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8717,7 +8982,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B20:J24"/>
+  <dimension ref="B20:J31"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
       <pane ySplit="21.0" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
@@ -8783,16 +9048,16 @@
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="51" t="s">
         <v>75</v>
-      </c>
-      <c r="C22" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="51" t="s">
-        <v>74</v>
       </c>
       <c r="F22" s="53" t="s">
         <v>40</v>
@@ -8800,24 +9065,24 @@
       <c r="G22" s="50" t="n">
         <v>1.0</v>
       </c>
-      <c r="H22" s="55"/>
-      <c r="I22" s="56" t="n">
+      <c r="H22" s="56" t="n">
         <v>1.0</v>
       </c>
-      <c r="J22" s="57"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="58"/>
     </row>
     <row r="23">
       <c r="B23" s="51" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="54" t="s">
-        <v>78</v>
+        <v>81</v>
+      </c>
+      <c r="C23" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="55" t="s">
+        <v>82</v>
       </c>
       <c r="E23" s="51" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F23" s="53" t="s">
         <v>40</v>
@@ -8825,24 +9090,24 @@
       <c r="G23" s="50" t="n">
         <v>1.0</v>
       </c>
-      <c r="H23" s="55"/>
-      <c r="I23" s="56" t="n">
+      <c r="H23" s="56" t="n">
         <v>1.0</v>
       </c>
-      <c r="J23" s="57"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="58"/>
     </row>
     <row r="24">
       <c r="B24" s="51" t="s">
-        <v>79</v>
-      </c>
-      <c r="C24" s="58" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="54" t="s">
-        <v>80</v>
+      <c r="D24" s="55" t="s">
+        <v>84</v>
       </c>
       <c r="E24" s="51" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F24" s="53" t="s">
         <v>40</v>
@@ -8850,11 +9115,186 @@
       <c r="G24" s="50" t="n">
         <v>1.0</v>
       </c>
-      <c r="H24" s="55" t="n">
+      <c r="H24" s="56" t="n">
         <v>1.0</v>
       </c>
-      <c r="I24" s="56"/>
-      <c r="J24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="58"/>
+    </row>
+    <row r="25">
+      <c r="B25" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H25" s="56" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I25" s="57"/>
+      <c r="J25" s="58"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="F26" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H26" s="56" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I26" s="57"/>
+      <c r="J26" s="58"/>
+    </row>
+    <row r="27">
+      <c r="B27" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H27" s="56"/>
+      <c r="I27" s="57" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J27" s="58"/>
+    </row>
+    <row r="28">
+      <c r="B28" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="G28" s="50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H28" s="56"/>
+      <c r="I28" s="57" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J28" s="58"/>
+    </row>
+    <row r="29">
+      <c r="B29" s="51" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="E29" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="G29" s="50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H29" s="56" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I29" s="57"/>
+      <c r="J29" s="58"/>
+    </row>
+    <row r="30">
+      <c r="B30" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="E30" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="G30" s="50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H30" s="56"/>
+      <c r="I30" s="57"/>
+      <c r="J30" s="58" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="E31" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="F31" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="G31" s="50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H31" s="56" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I31" s="57"/>
+      <c r="J31" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -8871,7 +9311,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="B20:I31"/>
+  <dimension ref="B20:I45"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
       <pane ySplit="21.0" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
@@ -8920,132 +9360,377 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="51" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="C22" s="50" t="n">
         <v>1.0</v>
       </c>
-      <c r="D22" s="55"/>
-      <c r="E22" s="56" t="n">
+      <c r="D22" s="56" t="n">
         <v>1.0</v>
       </c>
-      <c r="F22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="58"/>
       <c r="G22" s="59" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" s="51" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="C23" s="50" t="n">
         <v>1.0</v>
       </c>
-      <c r="D23" s="55"/>
-      <c r="E23" s="56" t="n">
+      <c r="D23" s="56" t="n">
         <v>1.0</v>
       </c>
-      <c r="F23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="58"/>
       <c r="G23" s="59" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="51" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="C24" s="50" t="n">
         <v>1.0</v>
       </c>
-      <c r="D24" s="55" t="n">
+      <c r="D24" s="56" t="n">
         <v>1.0</v>
       </c>
-      <c r="E24" s="56"/>
-      <c r="F24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="58"/>
       <c r="G24" s="59" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="I28" s="34" t="s">
-        <v>23</v>
+    <row r="25">
+      <c r="B25" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D25" s="56" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E25" s="57"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="59" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D26" s="56" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E26" s="57"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="59" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D27" s="56"/>
+      <c r="E27" s="57" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F27" s="58"/>
+      <c r="G27" s="59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" s="51" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D28" s="56"/>
+      <c r="E28" s="57" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F28" s="58"/>
+      <c r="G28" s="59" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="52" t="s">
-        <v>74</v>
-      </c>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="52" t="s">
-        <v>75</v>
-      </c>
-      <c r="I29" s="53" t="s">
-        <v>40</v>
+        <v>102</v>
+      </c>
+      <c r="C29" s="50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D29" s="56" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E29" s="57"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="59" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" s="51" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="I30" s="53" t="s">
-        <v>40</v>
+      <c r="C30" s="50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D30" s="56"/>
+      <c r="E30" s="57" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F30" s="58"/>
+      <c r="G30" s="59" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" s="51" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D31" s="56" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E31" s="57"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="59" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="42"/>
+      <c r="H35" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="I35" s="34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="60" t="s">
+        <v>79</v>
+      </c>
+      <c r="I36" s="54" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="52" t="s">
+      <c r="I37" s="54" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="I38" s="54" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="60" t="s">
+        <v>85</v>
+      </c>
+      <c r="I39" s="54" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="49"/>
+      <c r="H40" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="I40" s="54" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="I41" s="53" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" s="51" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="I42" s="53" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="I43" s="54" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="60" t="s">
-        <v>79</v>
-      </c>
-      <c r="I31" s="58" t="s">
+      <c r="C44" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" s="49"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="I44" s="53" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" s="51" t="s">
+        <v>103</v>
+      </c>
+      <c r="C45" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" s="49"/>
+      <c r="E45" s="49"/>
+      <c r="F45" s="49"/>
+      <c r="G45" s="49"/>
+      <c r="H45" s="60" t="s">
+        <v>94</v>
+      </c>
+      <c r="I45" s="54" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="14">
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C45:G45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9136,37 +9821,39 @@
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="51" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C22" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="54" t="s">
-        <v>83</v>
+      <c r="D22" s="55" t="s">
+        <v>104</v>
       </c>
       <c r="E22" s="50" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="F22" s="56" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="G22" s="57" t="n">
         <v>3.0</v>
       </c>
-      <c r="F22" s="55" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G22" s="56" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H22" s="57"/>
+      <c r="H22" s="58"/>
       <c r="I22" s="59" t="s">
         <v>71</v>
       </c>
       <c r="J22" s="50" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="K22" s="55" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="K22" s="56" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="L22" s="57" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M22" s="58" t="n">
         <v>1.0</v>
       </c>
-      <c r="L22" s="56" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="M22" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -9182,7 +9869,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E4"/>
+  <dimension ref="B2:E5"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
       <pane ySplit="2.0" state="frozen" topLeftCell="A3" activePane="bottomLeft"/>
@@ -9213,34 +9900,46 @@
     </row>
     <row r="3">
       <c r="B3" s="52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="E3" s="52" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="49"/>
       <c r="C4" s="52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>87</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="49"/>
+      <c r="C5" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" s="52" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" password="D541" scenarios="true" objects="true"/>
+  <sheetProtection sheet="true" password="AC8D" scenarios="true" objects="true"/>
   <mergeCells count="1">
-    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B3:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9299,13 +9998,13 @@
         <v>9</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>12</v>
       </c>
       <c r="H2" t="n" s="0">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -9325,7 +10024,7 @@
         <v>10</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>13</v>
@@ -9352,7 +10051,9 @@
       <c r="G4" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="H4" s="0"/>
+      <c r="H4" t="n" s="0">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s" s="0">
@@ -9371,13 +10072,13 @@
         <v>21</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>3.0</v>
+        <v>10.0</v>
       </c>
       <c r="G5" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H5" t="n" s="0">
-        <v>3.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -9462,20 +10163,20 @@
       </c>
       <c r="D20" s="50"/>
       <c r="H20" t="s" s="49">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I20" t="s" s="49">
         <v>40</v>
       </c>
       <c r="J20" s="50" t="n">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="K20" s="50" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="L20" s="50"/>
       <c r="P20" t="s" s="49">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Q20" t="s" s="49">
         <v>40</v>
@@ -9496,7 +10197,7 @@
       </c>
       <c r="D21" s="50"/>
       <c r="P21" s="49" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Q21" s="49" t="s">
         <v>40</v>
@@ -9506,6 +10207,27 @@
         <v>1.0</v>
       </c>
       <c r="T21" s="50"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D22" s="50"/>
+      <c r="P22" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q22" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="R22" s="50"/>
+      <c r="S22" s="50"/>
+      <c r="T22" s="50" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>

</xml_diff>